<commit_message>
2019-05-02 MRI project developing
</commit_message>
<xml_diff>
--- a/HH_Projects/01_Market_Risk_Indicator/Data_Files/Source_Files/ison_universe.xlsx
+++ b/HH_Projects/01_Market_Risk_Indicator/Data_Files/Source_Files/ison_universe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\GitHub Repository\HH_Codebase\HH_Projects\01_Market_Risk_Indicator\Data_Files\Source_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4678A8AE-9DE3-4FA5-9E76-FE24416B29D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF089B4C-71AA-48BF-851B-7AF2A719E0F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>RS</t>
   </si>
   <si>
-    <t>R0</t>
-  </si>
-  <si>
     <t>RE</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>CM</t>
   </si>
   <si>
-    <t>Cl</t>
-  </si>
-  <si>
     <t>BW</t>
   </si>
   <si>
@@ -452,6 +446,12 @@
   </si>
   <si>
     <t>Index Name</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>CI</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -905,22 +907,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -928,7 +930,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4">
         <v>25569</v>
@@ -946,7 +948,7 @@
         <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="4">
         <v>25569</v>
@@ -964,7 +966,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="4">
         <v>25569</v>
@@ -982,7 +984,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="4">
         <v>25569</v>
@@ -1000,7 +1002,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C6" s="4">
         <v>25569</v>
@@ -1018,7 +1020,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C7" s="4">
         <v>25569</v>
@@ -1036,7 +1038,7 @@
         <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8" s="4">
         <v>25569</v>
@@ -1054,7 +1056,7 @@
         <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" s="4">
         <v>25569</v>
@@ -1072,7 +1074,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" s="4">
         <v>25569</v>
@@ -1090,7 +1092,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" s="4">
         <v>25569</v>
@@ -1108,7 +1110,7 @@
         <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" s="4">
         <v>25569</v>
@@ -1126,7 +1128,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="4">
         <v>37043</v>
@@ -1135,7 +1137,7 @@
         <v>41300</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1147,7 +1149,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="4">
         <v>25569</v>
@@ -1165,7 +1167,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" s="4">
         <v>25569</v>
@@ -1183,7 +1185,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C16" s="4">
         <v>40324</v>
@@ -1201,7 +1203,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C17" s="4">
         <v>25569</v>
@@ -1219,7 +1221,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" s="4">
         <v>25569</v>
@@ -1237,7 +1239,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" s="4">
         <v>25569</v>
@@ -1255,7 +1257,7 @@
         <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20" s="4">
         <v>25569</v>
@@ -1273,7 +1275,7 @@
         <v>50</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21" s="4">
         <v>25569</v>
@@ -1291,7 +1293,7 @@
         <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" s="4">
         <v>35765</v>
@@ -1309,7 +1311,7 @@
         <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="4">
         <v>25569</v>
@@ -1327,7 +1329,7 @@
         <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C24" s="4">
         <v>25569</v>
@@ -1345,7 +1347,7 @@
         <v>50</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C25" s="4">
         <v>25569</v>
@@ -1363,7 +1365,7 @@
         <v>57</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="4">
         <v>41790</v>
@@ -1381,7 +1383,7 @@
         <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" s="4">
         <v>25569</v>
@@ -1390,7 +1392,7 @@
         <v>40503</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1402,7 +1404,7 @@
         <v>57</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C28" s="4">
         <v>25569</v>
@@ -1420,7 +1422,7 @@
         <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29" s="4">
         <v>25569</v>
@@ -1438,7 +1440,7 @@
         <v>57</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C30" s="4">
         <v>25569</v>
@@ -1456,7 +1458,7 @@
         <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="4">
         <v>34367</v>
@@ -1474,7 +1476,7 @@
         <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C32" s="4">
         <v>25569</v>
@@ -1492,7 +1494,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C33" s="4">
         <v>25569</v>
@@ -1510,7 +1512,7 @@
         <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C34" s="4">
         <v>25569</v>
@@ -1519,7 +1521,7 @@
         <v>37042</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F34" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1531,7 +1533,7 @@
         <v>57</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" s="4">
         <v>41605</v>
@@ -1549,7 +1551,7 @@
         <v>57</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36" s="4">
         <v>25569</v>
@@ -1567,7 +1569,7 @@
         <v>57</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" s="4">
         <v>25569</v>
@@ -1585,7 +1587,7 @@
         <v>57</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C38" s="4">
         <v>25569</v>
@@ -1594,7 +1596,7 @@
         <v>40323</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F38" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1606,7 +1608,7 @@
         <v>57</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C39" s="4">
         <v>25569</v>
@@ -1624,7 +1626,7 @@
         <v>57</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="4">
         <v>25569</v>
@@ -1633,7 +1635,7 @@
         <v>40503</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F40" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1645,7 +1647,7 @@
         <v>57</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C41" s="4">
         <v>25569</v>
@@ -1663,7 +1665,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="4">
         <v>25569</v>
@@ -1672,7 +1674,7 @@
         <v>40503</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F42" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1684,7 +1686,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="4">
         <v>25569</v>
@@ -1693,7 +1695,7 @@
         <v>41604</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F43" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1705,7 +1707,7 @@
         <v>57</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" s="4">
         <v>25569</v>
@@ -1723,7 +1725,7 @@
         <v>57</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45" s="4">
         <v>25569</v>
@@ -1741,7 +1743,7 @@
         <v>57</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" s="4">
         <v>25569</v>
@@ -1759,7 +1761,7 @@
         <v>57</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47" s="4">
         <v>25569</v>
@@ -1777,7 +1779,7 @@
         <v>57</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" s="4">
         <v>25569</v>
@@ -1786,7 +1788,7 @@
         <v>40503</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1798,7 +1800,7 @@
         <v>57</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="4">
         <v>42996</v>
@@ -1816,7 +1818,7 @@
         <v>57</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" s="4">
         <v>25569</v>
@@ -1834,7 +1836,7 @@
         <v>57</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" s="4">
         <v>25569</v>
@@ -1843,7 +1845,7 @@
         <v>35764</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F51" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1855,7 +1857,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C52" s="4">
         <v>41790</v>
@@ -1873,7 +1875,7 @@
         <v>57</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C53" s="4">
         <v>25569</v>
@@ -1891,7 +1893,7 @@
         <v>57</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" s="4">
         <v>25569</v>
@@ -1909,7 +1911,7 @@
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C55" s="4">
         <v>25569</v>
@@ -1927,7 +1929,7 @@
         <v>57</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C56" s="4">
         <v>25569</v>
@@ -1954,7 +1956,7 @@
         <v>42594</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F57" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1966,7 +1968,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C58" s="4">
         <v>25569</v>
@@ -1984,7 +1986,7 @@
         <v>219</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C59" s="4">
         <v>25569</v>
@@ -1993,7 +1995,7 @@
         <v>41789</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2005,7 +2007,7 @@
         <v>219</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C60" s="4">
         <v>25569</v>
@@ -2023,7 +2025,7 @@
         <v>219</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C61" s="4">
         <v>25569</v>
@@ -2041,7 +2043,7 @@
         <v>219</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C62" s="4">
         <v>40504</v>
@@ -2059,7 +2061,7 @@
         <v>219</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C63" s="4">
         <v>25569</v>
@@ -2077,7 +2079,7 @@
         <v>219</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C64" s="4">
         <v>40966</v>
@@ -2095,7 +2097,7 @@
         <v>219</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C65" s="4">
         <v>25569</v>
@@ -2113,7 +2115,7 @@
         <v>219</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C66" s="4">
         <v>25569</v>
@@ -2131,7 +2133,7 @@
         <v>219</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C67" s="4">
         <v>25569</v>
@@ -2149,7 +2151,7 @@
         <v>219</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C68" s="4">
         <v>25569</v>
@@ -2167,7 +2169,7 @@
         <v>219</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C69" s="4">
         <v>25569</v>
@@ -2185,7 +2187,7 @@
         <v>219</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C70" s="4">
         <v>25569</v>
@@ -2203,7 +2205,7 @@
         <v>219</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C71" s="4">
         <v>25569</v>
@@ -2221,7 +2223,7 @@
         <v>219</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="C72" s="4">
         <v>25569</v>
@@ -2239,7 +2241,7 @@
         <v>219</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C73" s="4">
         <v>25569</v>
@@ -2257,7 +2259,7 @@
         <v>219</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C74" s="4">
         <v>25569</v>
@@ -2266,7 +2268,7 @@
         <v>34366</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F74" s="8" t="str">
         <f t="shared" si="1"/>
@@ -2278,7 +2280,7 @@
         <v>219</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" s="4">
         <v>40966</v>
@@ -2296,7 +2298,7 @@
         <v>219</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C76" s="4">
         <v>25569</v>
@@ -2314,7 +2316,7 @@
         <v>219</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" s="4">
         <v>25569</v>
@@ -2332,7 +2334,7 @@
         <v>219</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" s="4">
         <v>25569</v>
@@ -2350,7 +2352,7 @@
         <v>219</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C79" s="4">
         <v>25569</v>
@@ -2368,7 +2370,7 @@
         <v>219</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C80" s="4">
         <v>40966</v>
@@ -2386,7 +2388,7 @@
         <v>219</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C81" s="4">
         <v>40966</v>
@@ -2404,7 +2406,7 @@
         <v>219</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C82" s="4">
         <v>25569</v>
@@ -2422,7 +2424,7 @@
         <v>219</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C83" s="4">
         <v>40966</v>
@@ -2440,7 +2442,7 @@
         <v>219</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C84" s="4">
         <v>25569</v>
@@ -2458,7 +2460,7 @@
         <v>219</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C85" s="4">
         <v>25569</v>
@@ -2476,7 +2478,7 @@
         <v>219</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C86" s="4">
         <v>25569</v>
@@ -2494,7 +2496,7 @@
         <v>219</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C87" s="4">
         <v>25569</v>
@@ -2512,7 +2514,7 @@
         <v>219</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C88" s="4">
         <v>25569</v>
@@ -2530,7 +2532,7 @@
         <v>219</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C89" s="4">
         <v>40966</v>
@@ -2548,7 +2550,7 @@
         <v>219</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C90" s="4">
         <v>25569</v>
@@ -2566,7 +2568,7 @@
         <v>219</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C91" s="4">
         <v>40966</v>
@@ -2584,7 +2586,7 @@
         <v>219</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C92" s="4">
         <v>40966</v>
@@ -2602,7 +2604,7 @@
         <v>219</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C93" s="4">
         <v>25569</v>
@@ -2620,7 +2622,7 @@
         <v>219</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C94" s="4">
         <v>40504</v>
@@ -2638,7 +2640,7 @@
         <v>219</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C95" s="4">
         <v>25569</v>
@@ -2656,7 +2658,7 @@
         <v>219</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C96" s="4">
         <v>40966</v>
@@ -2674,7 +2676,7 @@
         <v>219</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C97" s="4">
         <v>25569</v>
@@ -2692,7 +2694,7 @@
         <v>219</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C98" s="4">
         <v>25569</v>
@@ -2710,7 +2712,7 @@
         <v>219</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C99" s="4">
         <v>25569</v>
@@ -2728,7 +2730,7 @@
         <v>219</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C100" s="4">
         <v>25569</v>
@@ -2746,7 +2748,7 @@
         <v>219</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C101" s="4">
         <v>25569</v>
@@ -2764,7 +2766,7 @@
         <v>219</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C102" s="4">
         <v>25569</v>
@@ -2782,7 +2784,7 @@
         <v>219</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C103" s="4">
         <v>40504</v>
@@ -2800,7 +2802,7 @@
         <v>219</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C104" s="4">
         <v>25569</v>
@@ -2818,7 +2820,7 @@
         <v>219</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C105" s="4">
         <v>25569</v>
@@ -2836,7 +2838,7 @@
         <v>219</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C106" s="4">
         <v>25569</v>
@@ -2854,7 +2856,7 @@
         <v>219</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C107" s="4">
         <v>41605</v>
@@ -2872,7 +2874,7 @@
         <v>219</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C108" s="4">
         <v>25569</v>
@@ -2890,7 +2892,7 @@
         <v>219</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C109" s="4">
         <v>40966</v>
@@ -2908,7 +2910,7 @@
         <v>219</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C110" s="4">
         <v>25569</v>
@@ -2926,7 +2928,7 @@
         <v>219</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C111" s="4">
         <v>40966</v>
@@ -2944,7 +2946,7 @@
         <v>219</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C112" s="4">
         <v>40966</v>
@@ -2962,7 +2964,7 @@
         <v>219</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C113" s="4">
         <v>25569</v>
@@ -2980,7 +2982,7 @@
         <v>219</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C114" s="4">
         <v>25569</v>
@@ -2998,7 +3000,7 @@
         <v>219</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C115" s="4">
         <v>25569</v>
@@ -3016,7 +3018,7 @@
         <v>219</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C116" s="4">
         <v>25569</v>
@@ -3034,7 +3036,7 @@
         <v>219</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C117" s="4">
         <v>25569</v>
@@ -3052,7 +3054,7 @@
         <v>219</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C118" s="4">
         <v>25569</v>
@@ -3070,7 +3072,7 @@
         <v>219</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C119" s="4">
         <v>25569</v>
@@ -3088,7 +3090,7 @@
         <v>219</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C120" s="4">
         <v>25569</v>
@@ -3106,7 +3108,7 @@
         <v>219</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C121" s="4">
         <v>25569</v>
@@ -3124,7 +3126,7 @@
         <v>219</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C122" s="4">
         <v>25569</v>
@@ -3142,7 +3144,7 @@
         <v>219</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C123" s="4">
         <v>40504</v>
@@ -3151,7 +3153,7 @@
         <v>42995</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F123" s="8" t="str">
         <f t="shared" si="1"/>
@@ -3163,7 +3165,7 @@
         <v>219</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C124" s="4">
         <v>25569</v>
@@ -3181,7 +3183,7 @@
         <v>219</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C125" s="4">
         <v>25569</v>
@@ -3199,7 +3201,7 @@
         <v>219</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C126" s="4">
         <v>25569</v>
@@ -3208,7 +3210,7 @@
         <v>41789</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F126" s="8" t="str">
         <f t="shared" si="1"/>
@@ -3220,7 +3222,7 @@
         <v>219</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C127" s="4">
         <v>25569</v>
@@ -3238,7 +3240,7 @@
         <v>219</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="C128" s="4">
         <v>25569</v>

</xml_diff>